<commit_message>
Analyse - Maquettage, choix du framework
</commit_message>
<xml_diff>
--- a/2.Documentation/TB_Planning_Alt-Thibaud.xlsx
+++ b/2.Documentation/TB_Planning_Alt-Thibaud.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thibaud/Documents/HEIG/TB/3.Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thibaud/Documents/HEIG/TB/2.Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B3C94F-5331-6E44-988A-73CADE6D13E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA3113E0-5296-554C-9960-6D7510F72D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19680" xr2:uid="{7F10193E-5A70-1947-998D-BED32ABC87A4}"/>
   </bookViews>
@@ -16,9 +16,9 @@
     <sheet name="Planning &amp; Journal" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Planning &amp; Journal'!$C$1:$F$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Planning &amp; Journal'!$C$1:$F$15</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
   <si>
     <t>Tâche</t>
   </si>
@@ -109,6 +109,12 @@
   </si>
   <si>
     <t>À faire</t>
+  </si>
+  <si>
+    <t>Maquettage, choix du framework</t>
+  </si>
+  <si>
+    <t>Mise en place de Tailwind CSS</t>
   </si>
 </sst>
 </file>
@@ -308,7 +314,47 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -659,11 +705,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F44D29CA-69C2-AF43-823B-122E05E7E4AF}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I14" sqref="I14"/>
+      <selection pane="topRight" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -828,8 +874,8 @@
       <c r="B8" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>5</v>
+      <c r="C8" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="D8" s="11">
         <v>1</v>
@@ -846,61 +892,67 @@
       <c r="A9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>23</v>
+      <c r="B9" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="D9" s="11">
-        <v>125</v>
+        <v>3</v>
+      </c>
+      <c r="E9" s="11">
+        <v>3.5</v>
       </c>
       <c r="F9" s="8">
-        <f t="shared" ref="F9:F14" si="1">E9/D9</f>
-        <v>0</v>
+        <f>E9/D9</f>
+        <v>1.1666666666666667</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>25</v>
+      </c>
       <c r="C10" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="2">
-        <v>75</v>
-      </c>
-      <c r="E10" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="D10" s="11">
+        <v>1</v>
+      </c>
+      <c r="E10" s="11"/>
       <c r="F10" s="8">
-        <f t="shared" si="1"/>
+        <f>E10/D10</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="2"/>
+        <v>10</v>
+      </c>
       <c r="C11" s="11" t="s">
         <v>23</v>
       </c>
       <c r="D11" s="11">
-        <v>75</v>
-      </c>
-      <c r="E11" s="2"/>
+        <v>125</v>
+      </c>
       <c r="F11" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F11:F15" si="1">E11/D11</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="11" t="s">
         <v>23</v>
       </c>
       <c r="D12" s="2">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="8">
@@ -910,13 +962,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="11">
         <v>75</v>
       </c>
       <c r="E13" s="2"/>
@@ -926,54 +978,88 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="7"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="15"/>
-    </row>
-    <row r="15" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="13" t="s">
+      <c r="A14" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="2">
+        <v>100</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="2">
+        <v>75</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="7"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="15"/>
+    </row>
+    <row r="17" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="9"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="13">
-        <f>SUM(D2:D14)</f>
-        <v>459</v>
-      </c>
-      <c r="E15" s="13">
-        <f>SUM(E2:E14)</f>
-        <v>10</v>
-      </c>
-      <c r="F15" s="12">
-        <f>E15/D15</f>
-        <v>2.178649237472767E-2</v>
+      <c r="D17" s="13">
+        <f>SUM(D2:D16)</f>
+        <v>463</v>
+      </c>
+      <c r="E17" s="13">
+        <f>SUM(E2:E16)</f>
+        <v>13.5</v>
+      </c>
+      <c r="F17" s="12">
+        <f>E17/D17</f>
+        <v>2.9157667386609073E-2</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:F13" xr:uid="{7CC50BEF-57F7-764B-86D8-6AC718604565}"/>
+  <autoFilter ref="C1:F15" xr:uid="{7CC50BEF-57F7-764B-86D8-6AC718604565}"/>
   <mergeCells count="1">
-    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B16:F16"/>
   </mergeCells>
-  <conditionalFormatting sqref="C16:C1048576 C10:C13 C1:C8">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+  <conditionalFormatting sqref="C18:C1048576 C12:C15 C1:C10">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C6:C8">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+  <conditionalFormatting sqref="C6:C10">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C13 C15:C1048576">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C17:C1048576 C1:C15">
+    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Mise en place de TailwindCSS
</commit_message>
<xml_diff>
--- a/2.Documentation/TB_Planning_Alt-Thibaud.xlsx
+++ b/2.Documentation/TB_Planning_Alt-Thibaud.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thibaud/Documents/HEIG/TB/2.Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA3113E0-5296-554C-9960-6D7510F72D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB2F126-D90D-A343-8242-E65ACE3FD67A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19680" xr2:uid="{7F10193E-5A70-1947-998D-BED32ABC87A4}"/>
   </bookViews>
@@ -314,7 +314,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -347,16 +347,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -372,16 +362,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -709,7 +689,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C21" sqref="C21"/>
+      <selection pane="topRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -916,16 +896,18 @@
       <c r="B10" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>5</v>
+      <c r="C10" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="D10" s="11">
-        <v>1</v>
-      </c>
-      <c r="E10" s="11"/>
+        <v>0.5</v>
+      </c>
+      <c r="E10" s="11">
+        <v>0.5</v>
+      </c>
       <c r="F10" s="8">
         <f>E10/D10</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -933,7 +915,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="D11" s="11">
         <v>125</v>
@@ -1027,15 +1009,15 @@
       </c>
       <c r="D17" s="13">
         <f>SUM(D2:D16)</f>
-        <v>463</v>
+        <v>462.5</v>
       </c>
       <c r="E17" s="13">
         <f>SUM(E2:E16)</f>
-        <v>13.5</v>
+        <v>14</v>
       </c>
       <c r="F17" s="12">
         <f>E17/D17</f>
-        <v>2.9157667386609073E-2</v>
+        <v>3.027027027027027E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1043,24 +1025,34 @@
   <mergeCells count="1">
     <mergeCell ref="B16:F16"/>
   </mergeCells>
-  <conditionalFormatting sqref="C18:C1048576 C12:C15 C1:C10">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+  <conditionalFormatting sqref="C18:C1048576 C1:C8 C10:C15">
+    <cfRule type="cellIs" dxfId="5" priority="11" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C6:C10">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+  <conditionalFormatting sqref="C17:C1048576 C1:C8 C10:C15">
+    <cfRule type="containsText" dxfId="4" priority="9" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C8 C10:C1048576">
+    <cfRule type="containsText" dxfId="3" priority="8" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C17:C1048576 C1:C15">
-    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C1)))</formula>
+  <conditionalFormatting sqref="C9">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C9)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C1)))</formula>
+  <conditionalFormatting sqref="C9">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">

</xml_diff>

<commit_message>
State of the Art JS
</commit_message>
<xml_diff>
--- a/2.Documentation/TB_Planning_Alt-Thibaud.xlsx
+++ b/2.Documentation/TB_Planning_Alt-Thibaud.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thibaud/Documents/HEIG/TB/2.Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F84F1D-2AC0-BA46-BCE5-E8BFF03CC282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C9BA644-6673-114A-BA48-AE249F7FBCA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19680" xr2:uid="{7F10193E-5A70-1947-998D-BED32ABC87A4}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Planning &amp; Journal" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Planning &amp; Journal'!$C$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Planning &amp; Journal'!$C$1:$F$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
   <si>
     <t>Tâche</t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t>Maquette, squelette général</t>
+  </si>
+  <si>
+    <t>State of the Art JS, tour d'horizon</t>
+  </si>
+  <si>
+    <t>State of the Art JS, Frameworks JS</t>
   </si>
 </sst>
 </file>
@@ -320,7 +326,67 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -691,11 +757,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F44D29CA-69C2-AF43-823B-122E05E7E4AF}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J13" sqref="J13"/>
+      <selection pane="topRight" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -828,7 +894,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="8">
-        <f t="shared" ref="F6:F12" si="1">E6/D6</f>
+        <f t="shared" ref="F6:F14" si="1">E6/D6</f>
         <v>1</v>
       </c>
     </row>
@@ -962,145 +1028,217 @@
       <c r="A13" s="7" t="s">
         <v>10</v>
       </c>
+      <c r="B13" s="11" t="s">
+        <v>28</v>
+      </c>
       <c r="C13" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D13" s="11">
-        <v>110</v>
+        <v>4</v>
+      </c>
+      <c r="E13" s="11">
+        <v>2</v>
       </c>
       <c r="F13" s="8">
-        <f t="shared" ref="F13:F17" si="2">E13/D13</f>
-        <v>0</v>
+        <f t="shared" ref="F13" si="2">E13/D13</f>
+        <v>0.5</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>29</v>
+      </c>
       <c r="C14" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="2">
-        <v>75</v>
-      </c>
-      <c r="E14" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="D14" s="11">
+        <v>6</v>
+      </c>
+      <c r="E14" s="11">
+        <v>0</v>
+      </c>
       <c r="F14" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="2"/>
+        <v>10</v>
+      </c>
       <c r="C15" s="11" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="D15" s="11">
-        <v>75</v>
-      </c>
-      <c r="E15" s="2"/>
+        <v>100</v>
+      </c>
       <c r="F15" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="F15:F19" si="3">E15/D15</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="11" t="s">
         <v>23</v>
       </c>
       <c r="D16" s="2">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="11">
         <v>75</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="7"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="15"/>
-    </row>
-    <row r="19" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="13" t="s">
+      <c r="A18" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="2">
+        <v>100</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="8">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="2">
+        <v>75</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="8">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="7"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="15"/>
+    </row>
+    <row r="21" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="9"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="13">
-        <f>SUM(D2:D18)</f>
+      <c r="D21" s="13">
+        <f>SUM(D2:D20)</f>
         <v>449</v>
       </c>
-      <c r="E19" s="13">
-        <f>SUM(E2:E18)</f>
-        <v>17</v>
-      </c>
-      <c r="F19" s="12">
-        <f>E19/D19</f>
-        <v>3.7861915367483297E-2</v>
+      <c r="E21" s="13">
+        <f>SUM(E2:E20)</f>
+        <v>19</v>
+      </c>
+      <c r="F21" s="12">
+        <f>E21/D21</f>
+        <v>4.2316258351893093E-2</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:F17" xr:uid="{7CC50BEF-57F7-764B-86D8-6AC718604565}"/>
+  <autoFilter ref="C1:F19" xr:uid="{7CC50BEF-57F7-764B-86D8-6AC718604565}"/>
   <mergeCells count="1">
-    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B20:F20"/>
   </mergeCells>
-  <conditionalFormatting sqref="C20:C1048576 C1:C8 C10:C17">
-    <cfRule type="cellIs" dxfId="5" priority="11" operator="equal">
+  <conditionalFormatting sqref="C22:C1048576 C1:C8 C10:C12 C15:C19">
+    <cfRule type="cellIs" dxfId="11" priority="17" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C19:C1048576 C1:C8 C10:C17">
-    <cfRule type="containsText" dxfId="4" priority="9" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C21:C1048576 C1:C8 C10:C12 C15:C19">
+    <cfRule type="containsText" dxfId="10" priority="15" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C8 C10:C1048576">
-    <cfRule type="containsText" dxfId="3" priority="8" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C1:C8 C10:C12 C15:C1048576">
+    <cfRule type="containsText" dxfId="9" priority="14" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9">
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C14)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C14)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C9">
+  <conditionalFormatting sqref="C13">
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C9)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",C13)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C9">
+  <conditionalFormatting sqref="C13">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C9)))</formula>
+      <formula>NOT(ISERROR(SEARCH("à faire",C13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">

</xml_diff>

<commit_message>
Architecture, charte graphique, frameworks
</commit_message>
<xml_diff>
--- a/2.Documentation/TB_Planning_Alt-Thibaud.xlsx
+++ b/2.Documentation/TB_Planning_Alt-Thibaud.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thibaud/Documents/HEIG/TB/2.Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C314FA6A-CEF7-7C48-8D46-2AA6A62483AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905D9B7C-2C8C-1F4B-8FAE-63B6DAADD90D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="19680" xr2:uid="{7F10193E-5A70-1947-998D-BED32ABC87A4}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Planning &amp; Journal" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Planning &amp; Journal'!$C$1:$F$23</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Planning &amp; Journal'!$C$1:$F$24</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="35">
   <si>
     <t>Tâche</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>Applications web « State-of-the-Art », Frameworks</t>
+  </si>
+  <si>
+    <t>Charte graphique</t>
   </si>
 </sst>
 </file>
@@ -338,37 +341,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="27">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="24">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -919,11 +892,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F44D29CA-69C2-AF43-823B-122E05E7E4AF}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D14" sqref="D14"/>
+      <selection pane="topRight" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1056,7 +1029,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="8">
-        <f t="shared" ref="F6:F18" si="1">E6/D6</f>
+        <f t="shared" ref="F6:F19" si="1">E6/D6</f>
         <v>1</v>
       </c>
     </row>
@@ -1215,17 +1188,17 @@
         <v>31</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D14" s="11">
         <v>2</v>
       </c>
       <c r="E14" s="11">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="F14" s="8">
-        <f t="shared" ref="F14" si="2">E14/D14</f>
-        <v>0.25</v>
+        <f t="shared" ref="F14:F15" si="2">E14/D14</f>
+        <v>1.5</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1233,20 +1206,20 @@
         <v>10</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D15" s="11">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E15" s="11">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F15" s="8">
-        <f t="shared" si="1"/>
-        <v>0.66666666666666663</v>
+        <f t="shared" si="2"/>
+        <v>0.5</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1254,20 +1227,20 @@
         <v>10</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="11">
+        <v>6</v>
+      </c>
+      <c r="E16" s="11">
         <v>4</v>
-      </c>
-      <c r="E16" s="11">
-        <v>0.5</v>
       </c>
       <c r="F16" s="8">
         <f t="shared" si="1"/>
-        <v>0.125</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1275,7 +1248,7 @@
         <v>10</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>5</v>
@@ -1284,11 +1257,11 @@
         <v>4</v>
       </c>
       <c r="E17" s="11">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="F17" s="8">
-        <f t="shared" ref="F17" si="3">E17/D17</f>
-        <v>0.125</v>
+        <f t="shared" si="1"/>
+        <v>0.375</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1296,60 +1269,64 @@
         <v>10</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D18" s="11">
-        <v>10</v>
+        <v>4</v>
+      </c>
+      <c r="E18" s="11">
+        <v>0.5</v>
       </c>
       <c r="F18" s="8">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" ref="F18" si="3">E18/D18</f>
+        <v>0.125</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>10</v>
       </c>
+      <c r="B19" s="11" t="s">
+        <v>28</v>
+      </c>
       <c r="C19" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D19" s="11">
-        <v>87</v>
+        <v>10</v>
       </c>
       <c r="F19" s="8">
-        <f t="shared" ref="F19:F23" si="4">E19/D19</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="2"/>
+        <v>10</v>
+      </c>
       <c r="C20" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D20" s="2">
-        <v>75</v>
-      </c>
-      <c r="E20" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="D20" s="11">
+        <v>80</v>
+      </c>
       <c r="F20" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="F20:F24" si="4">E20/D20</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D21" s="11">
+      <c r="D21" s="2">
         <v>75</v>
       </c>
       <c r="E21" s="2"/>
@@ -1360,14 +1337,14 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="2">
-        <v>100</v>
+      <c r="D22" s="11">
+        <v>75</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="8">
@@ -1377,14 +1354,14 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="11" t="s">
         <v>23</v>
       </c>
       <c r="D23" s="2">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="8">
@@ -1393,140 +1370,157 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="7"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="15"/>
-    </row>
-    <row r="25" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="13" t="s">
+      <c r="A24" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="2">
+        <v>75</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="8">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="7"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="15"/>
+    </row>
+    <row r="26" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="9"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="13">
-        <f>SUM(D2:D24)</f>
-        <v>454</v>
-      </c>
-      <c r="E25" s="13">
-        <f>SUM(E2:E24)</f>
-        <v>25.5</v>
-      </c>
-      <c r="F25" s="12">
-        <f>E25/D25</f>
-        <v>5.6167400881057268E-2</v>
+      <c r="D26" s="13">
+        <f>SUM(D2:D25)</f>
+        <v>449</v>
+      </c>
+      <c r="E26" s="13">
+        <f>SUM(E2:E25)</f>
+        <v>30</v>
+      </c>
+      <c r="F26" s="12">
+        <f>E26/D26</f>
+        <v>6.6815144766147E-2</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:F23" xr:uid="{7CC50BEF-57F7-764B-86D8-6AC718604565}"/>
+  <autoFilter ref="C1:F24" xr:uid="{7CC50BEF-57F7-764B-86D8-6AC718604565}"/>
   <mergeCells count="1">
-    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:F25"/>
   </mergeCells>
-  <conditionalFormatting sqref="C26:C1048576 C1:C8 C10:C12 C19:C23">
-    <cfRule type="cellIs" dxfId="20" priority="26" operator="equal">
+  <conditionalFormatting sqref="C27:C1048576 C1:C8 C10:C12 C20:C24">
+    <cfRule type="cellIs" dxfId="23" priority="29" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C25:C1048576 C1:C8 C10:C12 C19:C23">
-    <cfRule type="containsText" dxfId="19" priority="24" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C26:C1048576 C1:C8 C10:C12 C20:C24">
+    <cfRule type="containsText" dxfId="22" priority="27" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C8 C10:C12 C19:C1048576">
-    <cfRule type="containsText" dxfId="18" priority="23" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C1:C8 C10:C12 C20:C1048576">
+    <cfRule type="containsText" dxfId="21" priority="26" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
+    <cfRule type="cellIs" dxfId="20" priority="21" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9">
+    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9">
+    <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16">
     <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C9">
+  <conditionalFormatting sqref="C16">
     <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C9)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C9">
+      <formula>NOT(ISERROR(SEARCH("En cours",C16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16">
     <cfRule type="containsText" dxfId="15" priority="16" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C9)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C15">
-    <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C15">
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C15)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C15">
-    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C15)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14">
+      <formula>NOT(ISERROR(SEARCH("à faire",C16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17 C19">
     <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C14">
+  <conditionalFormatting sqref="C17 C19">
     <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C14)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14">
+      <formula>NOT(ISERROR(SEARCH("En cours",C17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17 C19">
     <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C14)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C16 C18">
+      <formula>NOT(ISERROR(SEARCH("à faire",C17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13:C14">
     <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C16 C18">
+  <conditionalFormatting sqref="C13:C14">
     <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C16)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C16 C18">
+      <formula>NOT(ISERROR(SEARCH("En cours",C13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13:C14">
     <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C16)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C13">
+      <formula>NOT(ISERROR(SEARCH("à faire",C13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18">
     <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C13">
+  <conditionalFormatting sqref="C18">
     <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C13)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C13">
+      <formula>NOT(ISERROR(SEARCH("En cours",C18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18">
     <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C13)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C17">
-    <cfRule type="cellIs" dxfId="26" priority="3" operator="equal">
+      <formula>NOT(ISERROR(SEARCH("à faire",C18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C17">
-    <cfRule type="containsText" dxfId="25" priority="2" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C17)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C17">
-    <cfRule type="containsText" dxfId="24" priority="1" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C17)))</formula>
+  <conditionalFormatting sqref="C15">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">

</xml_diff>

<commit_message>
Refactorisation de la documentation
</commit_message>
<xml_diff>
--- a/2.Documentation/TB_Planning_Alt-Thibaud.xlsx
+++ b/2.Documentation/TB_Planning_Alt-Thibaud.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thibaud/Documents/HEIG/TB/2.Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D4A5356-1422-E54E-8067-A6E380F40ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42CF34E4-28AE-D440-BC90-84B70F9B20F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="19680" xr2:uid="{7F10193E-5A70-1947-998D-BED32ABC87A4}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Planning &amp; Journal" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Planning &amp; Journal'!$C$1:$F$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Planning &amp; Journal'!$C$1:$F$26</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="37">
   <si>
     <t>Tâche</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>Maquette, page de login</t>
+  </si>
+  <si>
+    <t>Refactorisation générale de la documentation</t>
   </si>
 </sst>
 </file>
@@ -895,11 +898,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F44D29CA-69C2-AF43-823B-122E05E7E4AF}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K19" sqref="K19"/>
+      <selection pane="topRight" activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -966,11 +969,11 @@
         <v>1</v>
       </c>
       <c r="E3" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3" s="8">
         <f t="shared" ref="F3:F5" si="0">E3/D3</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -987,11 +990,11 @@
         <v>1</v>
       </c>
       <c r="E4" s="2">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="F4" s="8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1008,11 +1011,11 @@
         <v>2</v>
       </c>
       <c r="E5" s="11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F5" s="8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1029,11 +1032,11 @@
         <v>1</v>
       </c>
       <c r="E6" s="11">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="F6" s="8">
-        <f t="shared" ref="F6:F20" si="1">E6/D6</f>
-        <v>1</v>
+        <f t="shared" ref="F6:F21" si="1">E6/D6</f>
+        <v>1.5</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1113,11 +1116,11 @@
         <v>1</v>
       </c>
       <c r="E10" s="11">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="F10" s="8">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1212,17 +1215,17 @@
         <v>31</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D15" s="11">
         <v>2</v>
       </c>
       <c r="E15" s="11">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="F15" s="8">
         <f t="shared" si="2"/>
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1233,7 +1236,7 @@
         <v>34</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D16" s="11">
         <v>6</v>
@@ -1254,7 +1257,7 @@
         <v>32</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D17" s="11">
         <v>4</v>
@@ -1275,7 +1278,7 @@
         <v>33</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D18" s="11">
         <v>4</v>
@@ -1296,7 +1299,7 @@
         <v>28</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D19" s="11">
         <v>10</v>
@@ -1323,54 +1326,58 @@
         <v>2</v>
       </c>
       <c r="E20">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="F20" s="8">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>10</v>
       </c>
+      <c r="B21" s="11" t="s">
+        <v>36</v>
+      </c>
       <c r="C21" s="11" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D21" s="11">
-        <v>80</v>
+        <v>3</v>
+      </c>
+      <c r="E21">
+        <v>3</v>
       </c>
       <c r="F21" s="8">
-        <f t="shared" ref="F21:F25" si="4">E21/D21</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B22" s="2"/>
+        <v>10</v>
+      </c>
       <c r="C22" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D22" s="2">
+        <v>5</v>
+      </c>
+      <c r="D22" s="11">
         <v>75</v>
       </c>
-      <c r="E22" s="2"/>
       <c r="F22" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="F22:F26" si="4">E22/D22</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="11">
+      <c r="D23" s="2">
         <v>75</v>
       </c>
       <c r="E23" s="2"/>
@@ -1381,14 +1388,14 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="2">
-        <v>100</v>
+      <c r="D24" s="11">
+        <v>75</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="8">
@@ -1398,14 +1405,14 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="11" t="s">
         <v>23</v>
       </c>
       <c r="D25" s="2">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="8">
@@ -1414,48 +1421,65 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="7"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="15"/>
-    </row>
-    <row r="27" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="9"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="13" t="s">
+      <c r="A26" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="2">
+        <v>75</v>
+      </c>
+      <c r="E26" s="2"/>
+      <c r="F26" s="8">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="7"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="15"/>
+    </row>
+    <row r="28" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="9"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D27" s="13">
-        <f>SUM(D2:D26)</f>
-        <v>451</v>
-      </c>
-      <c r="E27" s="13">
-        <f>SUM(E2:E26)</f>
-        <v>42</v>
-      </c>
-      <c r="F27" s="12">
-        <f>E27/D27</f>
-        <v>9.3126385809312637E-2</v>
+      <c r="D28" s="13">
+        <f>SUM(D2:D27)</f>
+        <v>449</v>
+      </c>
+      <c r="E28" s="13">
+        <f>SUM(E2:E27)</f>
+        <v>49.5</v>
+      </c>
+      <c r="F28" s="12">
+        <f>E28/D28</f>
+        <v>0.11024498886414254</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:F25" xr:uid="{7CC50BEF-57F7-764B-86D8-6AC718604565}"/>
+  <autoFilter ref="C1:F26" xr:uid="{7CC50BEF-57F7-764B-86D8-6AC718604565}"/>
   <mergeCells count="1">
-    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
   </mergeCells>
-  <conditionalFormatting sqref="C28:C1048576 C1:C8 C10:C12 C21:C25">
+  <conditionalFormatting sqref="C29:C1048576 C1:C8 C10:C12 C22:C26">
     <cfRule type="cellIs" dxfId="23" priority="32" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C27:C1048576 C1:C8 C10:C12 C21:C25">
+  <conditionalFormatting sqref="C28:C1048576 C1:C8 C10:C12 C22:C26">
     <cfRule type="containsText" dxfId="22" priority="30" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C8 C10:C12 C21:C1048576">
+  <conditionalFormatting sqref="C1:C8 C10:C12 C22:C1048576">
     <cfRule type="containsText" dxfId="21" priority="29" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C1)))</formula>
     </cfRule>
@@ -1475,92 +1499,32 @@
       <formula>NOT(ISERROR(SEARCH("à faire",C9)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C16">
-    <cfRule type="cellIs" dxfId="17" priority="21" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C16">
-    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C16)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C16">
-    <cfRule type="containsText" dxfId="15" priority="19" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C16)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C17 C19">
-    <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C17 C19">
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C17)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C17 C19">
-    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C17)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C13:C14">
+  <conditionalFormatting sqref="C13:C19">
     <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C13:C14">
+  <conditionalFormatting sqref="C13:C19">
     <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C13)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C13:C14">
+  <conditionalFormatting sqref="C13:C19">
     <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C13)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C18">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C18">
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C18">
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C15">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C15">
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C15)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C15">
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C15)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C20">
+  <conditionalFormatting sqref="C20:C21">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C20">
+  <conditionalFormatting sqref="C20:C21">
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C20">
+  <conditionalFormatting sqref="C20:C21">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C20)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
Système de gestion de base de données
</commit_message>
<xml_diff>
--- a/2.Documentation/TB_Planning_Alt-Thibaud.xlsx
+++ b/2.Documentation/TB_Planning_Alt-Thibaud.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thibaud/Documents/HEIG/TB/2.Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42CF34E4-28AE-D440-BC90-84B70F9B20F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3447326-95F4-EF4E-A7CF-0CB4FC132567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="19680" xr2:uid="{7F10193E-5A70-1947-998D-BED32ABC87A4}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Planning &amp; Journal" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Planning &amp; Journal'!$C$1:$F$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Planning &amp; Journal'!$C$1:$F$27</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="38">
   <si>
     <t>Tâche</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>Refactorisation générale de la documentation</t>
+  </si>
+  <si>
+    <t>Système de gestion de base de données</t>
   </si>
 </sst>
 </file>
@@ -347,127 +350,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="24">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -898,11 +781,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F44D29CA-69C2-AF43-823B-122E05E7E4AF}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H21" sqref="H21"/>
+      <selection pane="topRight" activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1035,7 +918,7 @@
         <v>1.5</v>
       </c>
       <c r="F6" s="8">
-        <f t="shared" ref="F6:F21" si="1">E6/D6</f>
+        <f t="shared" ref="F6:F22" si="1">E6/D6</f>
         <v>1.5</v>
       </c>
     </row>
@@ -1358,43 +1241,47 @@
       <c r="A22" s="7" t="s">
         <v>10</v>
       </c>
+      <c r="B22" s="11" t="s">
+        <v>37</v>
+      </c>
       <c r="C22" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D22" s="11">
-        <v>75</v>
+        <v>10</v>
+      </c>
+      <c r="E22">
+        <v>9</v>
       </c>
       <c r="F22" s="8">
-        <f t="shared" ref="F22:F26" si="4">E22/D22</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.9</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" s="2"/>
+        <v>10</v>
+      </c>
       <c r="C23" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D23" s="2">
+        <v>5</v>
+      </c>
+      <c r="D23" s="11">
         <v>75</v>
       </c>
-      <c r="E23" s="2"/>
       <c r="F23" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="F23:F27" si="4">E23/D23</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="11">
+      <c r="D24" s="2">
         <v>75</v>
       </c>
       <c r="E24" s="2"/>
@@ -1405,14 +1292,14 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="2">
-        <v>100</v>
+      <c r="D25" s="11">
+        <v>75</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="8">
@@ -1422,14 +1309,14 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="11" t="s">
         <v>23</v>
       </c>
       <c r="D26" s="2">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="8">
@@ -1438,79 +1325,96 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="7"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="15"/>
-    </row>
-    <row r="28" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="9"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="13" t="s">
+      <c r="A27" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" s="2">
+        <v>75</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="F27" s="8">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="7"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="15"/>
+    </row>
+    <row r="29" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="9"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D28" s="13">
-        <f>SUM(D2:D27)</f>
-        <v>449</v>
-      </c>
-      <c r="E28" s="13">
-        <f>SUM(E2:E27)</f>
-        <v>49.5</v>
-      </c>
-      <c r="F28" s="12">
-        <f>E28/D28</f>
-        <v>0.11024498886414254</v>
+      <c r="D29" s="13">
+        <f>SUM(D2:D28)</f>
+        <v>459</v>
+      </c>
+      <c r="E29" s="13">
+        <f>SUM(E2:E28)</f>
+        <v>58.5</v>
+      </c>
+      <c r="F29" s="12">
+        <f>E29/D29</f>
+        <v>0.12745098039215685</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:F26" xr:uid="{7CC50BEF-57F7-764B-86D8-6AC718604565}"/>
+  <autoFilter ref="C1:F27" xr:uid="{7CC50BEF-57F7-764B-86D8-6AC718604565}"/>
   <mergeCells count="1">
-    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B28:F28"/>
   </mergeCells>
-  <conditionalFormatting sqref="C29:C1048576 C1:C8 C10:C12 C22:C26">
-    <cfRule type="cellIs" dxfId="23" priority="32" operator="equal">
+  <conditionalFormatting sqref="C30:C1048576 C1:C8 C10:C12 C22:C27">
+    <cfRule type="cellIs" dxfId="11" priority="32" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C28:C1048576 C1:C8 C10:C12 C22:C26">
-    <cfRule type="containsText" dxfId="22" priority="30" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C29:C1048576 C1:C8 C10:C12 C22:C27">
+    <cfRule type="containsText" dxfId="10" priority="30" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C8 C10:C12 C22:C1048576">
-    <cfRule type="containsText" dxfId="21" priority="29" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="9" priority="29" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="20" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="24" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="7" priority="23" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="containsText" dxfId="18" priority="22" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="6" priority="22" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13:C19">
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="12" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13:C19">
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="4" priority="11" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13:C19">
-    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="3" priority="10" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C13)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Multilinguisme + User stories
</commit_message>
<xml_diff>
--- a/2.Documentation/TB_Planning_Alt-Thibaud.xlsx
+++ b/2.Documentation/TB_Planning_Alt-Thibaud.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thibaud/Documents/HEIG/TB/2.Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3447326-95F4-EF4E-A7CF-0CB4FC132567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE696B9-92B1-DD4E-9308-E4371E720F0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="19680" xr2:uid="{7F10193E-5A70-1947-998D-BED32ABC87A4}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Planning &amp; Journal" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Planning &amp; Journal'!$C$1:$F$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Planning &amp; Journal'!$C$1:$F$31</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="41">
   <si>
     <t>Tâche</t>
   </si>
@@ -151,6 +151,15 @@
   </si>
   <si>
     <t>Système de gestion de base de données</t>
+  </si>
+  <si>
+    <t>Multilinguisme</t>
+  </si>
+  <si>
+    <t>User stories</t>
+  </si>
+  <si>
+    <t>Mise en place SCRUM (Trello)</t>
   </si>
 </sst>
 </file>
@@ -350,7 +359,127 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="24">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -781,11 +910,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F44D29CA-69C2-AF43-823B-122E05E7E4AF}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H22" sqref="H22"/>
+      <selection pane="topRight" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -918,7 +1047,7 @@
         <v>1.5</v>
       </c>
       <c r="F6" s="8">
-        <f t="shared" ref="F6:F22" si="1">E6/D6</f>
+        <f t="shared" ref="F6:F23" si="1">E6/D6</f>
         <v>1.5</v>
       </c>
     </row>
@@ -1182,7 +1311,7 @@
         <v>28</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D19" s="11">
         <v>10</v>
@@ -1224,17 +1353,17 @@
         <v>36</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D21" s="11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E21">
         <v>3</v>
       </c>
       <c r="F21" s="8">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1245,192 +1374,319 @@
         <v>37</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D22" s="11">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E22">
         <v>9</v>
       </c>
       <c r="F22" s="8">
         <f t="shared" si="1"/>
-        <v>0.9</v>
+        <v>1.125</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>10</v>
       </c>
+      <c r="B23" s="11" t="s">
+        <v>38</v>
+      </c>
       <c r="C23" s="11" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D23" s="11">
-        <v>75</v>
+        <v>3</v>
+      </c>
+      <c r="E23">
+        <v>2</v>
       </c>
       <c r="F23" s="8">
-        <f t="shared" ref="F23:F27" si="4">E23/D23</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B24" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>39</v>
+      </c>
       <c r="C24" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D24" s="2">
-        <v>75</v>
-      </c>
-      <c r="E24" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="D24" s="11">
+        <v>3</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
       <c r="F24" s="8">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" ref="F24:F25" si="4">E24/D24</f>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>40</v>
+      </c>
       <c r="C25" s="11" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="D25" s="11">
-        <v>75</v>
-      </c>
-      <c r="E25" s="2"/>
+        <v>2</v>
+      </c>
       <c r="F25" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D26" s="2">
-        <v>100</v>
-      </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="8">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
+      <c r="A26" s="7"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="F26" s="8"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="11">
+        <v>60</v>
+      </c>
+      <c r="F27" s="8">
+        <f t="shared" ref="F27:F31" si="5">E27/D27</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" s="2">
+        <v>75</v>
+      </c>
+      <c r="E28" s="2"/>
+      <c r="F28" s="8">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D29" s="11">
+        <v>75</v>
+      </c>
+      <c r="E29" s="2"/>
+      <c r="F29" s="8">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" s="2">
+        <v>100</v>
+      </c>
+      <c r="E30" s="2"/>
+      <c r="F30" s="8">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="11" t="s">
+      <c r="B31" s="2"/>
+      <c r="C31" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D31" s="2">
         <v>75</v>
       </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="8">
-        <f t="shared" si="4"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="8">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="7"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="15"/>
-    </row>
-    <row r="29" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="9"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="13" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="7"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="15"/>
+    </row>
+    <row r="33" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="9"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="13">
-        <f>SUM(D2:D28)</f>
-        <v>459</v>
-      </c>
-      <c r="E29" s="13">
-        <f>SUM(E2:E28)</f>
-        <v>58.5</v>
-      </c>
-      <c r="F29" s="12">
-        <f>E29/D29</f>
-        <v>0.12745098039215685</v>
+      <c r="D33" s="13">
+        <f>SUM(D2:D32)</f>
+        <v>451</v>
+      </c>
+      <c r="E33" s="13">
+        <f>SUM(E2:E32)</f>
+        <v>62.5</v>
+      </c>
+      <c r="F33" s="12">
+        <f>E33/D33</f>
+        <v>0.13858093126385809</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:F27" xr:uid="{7CC50BEF-57F7-764B-86D8-6AC718604565}"/>
+  <autoFilter ref="C1:F31" xr:uid="{7CC50BEF-57F7-764B-86D8-6AC718604565}"/>
   <mergeCells count="1">
-    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B32:F32"/>
   </mergeCells>
-  <conditionalFormatting sqref="C30:C1048576 C1:C8 C10:C12 C22:C27">
-    <cfRule type="cellIs" dxfId="11" priority="32" operator="equal">
+  <conditionalFormatting sqref="C34:C1048576 C1:C8 C10:C12 C27:C31">
+    <cfRule type="cellIs" dxfId="23" priority="44" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C29:C1048576 C1:C8 C10:C12 C22:C27">
-    <cfRule type="containsText" dxfId="10" priority="30" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C33:C1048576 C1:C8 C10:C12 C27:C31">
+    <cfRule type="containsText" dxfId="22" priority="42" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C8 C10:C12 C22:C1048576">
-    <cfRule type="containsText" dxfId="9" priority="29" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C1:C8 C10:C12 C27:C1048576">
+    <cfRule type="containsText" dxfId="21" priority="41" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="8" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="36" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="containsText" dxfId="7" priority="23" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="19" priority="35" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="containsText" dxfId="6" priority="22" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="18" priority="34" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C9)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C13:C19">
-    <cfRule type="cellIs" dxfId="5" priority="12" operator="equal">
+  <conditionalFormatting sqref="C13:C18">
+    <cfRule type="cellIs" dxfId="17" priority="24" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C13:C19">
-    <cfRule type="containsText" dxfId="4" priority="11" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C13:C18">
+    <cfRule type="containsText" dxfId="16" priority="23" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C13)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C13:C19">
-    <cfRule type="containsText" dxfId="3" priority="10" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C13:C18">
+    <cfRule type="containsText" dxfId="15" priority="22" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C13)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C20:C21">
+  <conditionalFormatting sqref="C20 C22:C23">
+    <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20 C22:C23">
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20 C22:C23">
+    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C24">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C24">
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C24)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C24">
+    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C24)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C21">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C21">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C21)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C21">
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C21)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C25:C26">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C25:C26">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C25)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C25:C26">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C25)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C20:C21">
+  <conditionalFormatting sqref="C19">
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C20)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C20:C21">
+      <formula>NOT(ISERROR(SEARCH("En cours",C19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C20)))</formula>
+      <formula>NOT(ISERROR(SEARCH("à faire",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">

</xml_diff>